<commit_message>
Change names of tabs in Eldata.xls
The names of tabs has been changed so that we can include a tab for
elasticity and a tab for productivity for each different type of
production structure
</commit_message>
<xml_diff>
--- a/documentation/templates/Eldata.xlsx
+++ b/documentation/templates/Eldata.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet name="elasFU" sheetId="5" r:id="rId1"/>
     <sheet name="elasTRADE" sheetId="8" r:id="rId2"/>
-    <sheet name="elasPROD" sheetId="9" r:id="rId3"/>
-    <sheet name="FPROD" sheetId="10" r:id="rId4"/>
+    <sheet name="elasKL" sheetId="9" r:id="rId3"/>
+    <sheet name="prodKL" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>

</xml_diff>

<commit_message>
Finalize production module KL-E
- added comments in the code
- made consistent with other modules
- input file with elasticities is adjusted
</commit_message>
<xml_diff>
--- a/documentation/templates/Eldata.xlsx
+++ b/documentation/templates/Eldata.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU" sheetId="5" r:id="rId1"/>
     <sheet name="elasTRADE" sheetId="8" r:id="rId2"/>
     <sheet name="elasKL" sheetId="9" r:id="rId3"/>
     <sheet name="prodKL" sheetId="10" r:id="rId4"/>
+    <sheet name="elasKL-E" sheetId="11" r:id="rId5"/>
+    <sheet name="prodKL-E" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>elasIU_DM</t>
   </si>
@@ -92,6 +94,15 @@
   </si>
   <si>
     <t>ind5</t>
+  </si>
+  <si>
+    <t>elasKLE</t>
+  </si>
+  <si>
+    <t>elasE</t>
+  </si>
+  <si>
+    <t>ENER</t>
   </si>
 </sst>
 </file>
@@ -434,9 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -484,9 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -632,9 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -770,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -903,4 +908,288 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add demand module with LES-CES function for household
The demand module is almost the same as CES demand module, only
calibration and demand function for households is changed.
</commit_message>
<xml_diff>
--- a/documentation/templates/Eldata.xlsx
+++ b/documentation/templates/Eldata.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780"/>
   </bookViews>
   <sheets>
-    <sheet name="elasFU" sheetId="5" r:id="rId1"/>
-    <sheet name="elasTRADE" sheetId="8" r:id="rId2"/>
-    <sheet name="elasKL" sheetId="9" r:id="rId3"/>
-    <sheet name="prodKL" sheetId="10" r:id="rId4"/>
-    <sheet name="elasKL-E" sheetId="11" r:id="rId5"/>
-    <sheet name="prodKL-E" sheetId="12" r:id="rId6"/>
+    <sheet name="elasFU_CES" sheetId="5" r:id="rId1"/>
+    <sheet name="elasFU_LES" sheetId="13" r:id="rId2"/>
+    <sheet name="elasTRADE" sheetId="8" r:id="rId3"/>
+    <sheet name="elasKL" sheetId="9" r:id="rId4"/>
+    <sheet name="prodKL" sheetId="10" r:id="rId5"/>
+    <sheet name="elasKL-E" sheetId="11" r:id="rId6"/>
+    <sheet name="prodKL-E" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>elasIU_DM</t>
   </si>
@@ -103,6 +104,12 @@
   </si>
   <si>
     <t>ENER</t>
+  </si>
+  <si>
+    <t>elasINC</t>
+  </si>
+  <si>
+    <t>frisch</t>
   </si>
 </sst>
 </file>
@@ -445,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -491,9 +498,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -635,7 +700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
@@ -771,7 +836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
@@ -910,7 +975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -1052,11 +1117,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>